<commit_message>
All updates to have convergent steady state model
</commit_message>
<xml_diff>
--- a/Data/data_waterlevels/obs/02_Model_bores_elevations.xlsx
+++ b/Data/data_waterlevels/obs/02_Model_bores_elevations.xlsx
@@ -1498,9 +1498,7 @@
         <v>115.463555338</v>
       </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>209.7193908691406</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">

</xml_diff>